<commit_message>
* [LocTT] update 3 field export Main2
</commit_message>
<xml_diff>
--- a/KhoanNhaTrang/Template/TemplateMain2.xlsx
+++ b/KhoanNhaTrang/Template/TemplateMain2.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t xml:space="preserve">Water Pressure Report</t>
   </si>
@@ -88,7 +88,13 @@
     <t xml:space="preserve">{tab1.flowrate}</t>
   </si>
   <si>
+    <t xml:space="preserve">{tab1.tfluid}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{tab1.pressure}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{tab1.wc}</t>
   </si>
   <si>
     <t xml:space="preserve">{par2.endtime}</t>
@@ -236,10 +242,10 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.87890625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.22"/>
@@ -365,11 +371,15 @@
       <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="D18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="0"/>
+        <v>22</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -378,22 +388,22 @@
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -403,7 +413,7 @@
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>